<commit_message>
funcionalidades de la 61 a la 70 agregadas
</commit_message>
<xml_diff>
--- a/Informe Semana 7.xlsx
+++ b/Informe Semana 7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MISO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresmartincantorurrego/Desktop/MAESTRIA/SEMESTRE 1/CICLO 2/PRUEBAS AUTOMATIZADAS /proyecto/semana5-pruebas-automatizadas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AA31FE9-53DB-4529-B638-EA069C436854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44541E8D-7BA6-9B49-B939-32A16125CACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{21504B3F-757C-4B36-B248-990E3DFEA9E7}"/>
+    <workbookView xWindow="540" yWindow="500" windowWidth="37860" windowHeight="21100" xr2:uid="{21504B3F-757C-4B36-B248-990E3DFEA9E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="89">
   <si>
     <t>ID</t>
   </si>
@@ -227,6 +227,111 @@
       </rPr>
       <t>Al poder hacer el loop, se facilitó la ejecución de escenarios diferentes en un solo script, por eso se agrupan y no existen los scripts del 92 al 100</t>
     </r>
+  </si>
+  <si>
+    <t>Martin Cantor</t>
+  </si>
+  <si>
+    <t>Creacion de Miembros</t>
+  </si>
+  <si>
+    <t>Escenario-prueba71.js</t>
+  </si>
+  <si>
+    <t>Escenario-prueba72.js</t>
+  </si>
+  <si>
+    <t>Escenario-prueba73.js</t>
+  </si>
+  <si>
+    <t>Escenario-prueba74.js</t>
+  </si>
+  <si>
+    <t>Escenario-prueba75.js</t>
+  </si>
+  <si>
+    <t>Escenario-prueba76.js</t>
+  </si>
+  <si>
+    <t>Escenario-prueba77.js</t>
+  </si>
+  <si>
+    <t>Escenario-prueba78.js</t>
+  </si>
+  <si>
+    <t>Escenario-prueba79.js</t>
+  </si>
+  <si>
+    <t>Escenario-prueba80.js</t>
+  </si>
+  <si>
+    <t>Escenario-prueba91.js</t>
+  </si>
+  <si>
+    <t>Escenario-prueba61-70.js</t>
+  </si>
+  <si>
+    <t>Creacion de miembro valido</t>
+  </si>
+  <si>
+    <t>Creacion de miembro sin correo</t>
+  </si>
+  <si>
+    <t>Creacion de miembro sin nombre</t>
+  </si>
+  <si>
+    <t>Creacion de miembro con correo  repetido</t>
+  </si>
+  <si>
+    <t>Creacion de miembro sin Labels</t>
+  </si>
+  <si>
+    <t>Creacion de miembro con Note mayor a 500 caracteres</t>
+  </si>
+  <si>
+    <t>Creacion de miembro con Note vacio</t>
+  </si>
+  <si>
+    <t>Creacion de miembro y luego eliminarlo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set a-priori generado con Mockaroo, descargado y adaptado
+En la colección de datos (archivo de fixtures creacion_miembro.json) se tiene un registro por cada prueba a realizar y el resultado esperado de cada prueba, el script recore los datos y hace las 10 pruebas.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Al poder hacer el loop, se facilitó la ejecución de escenarios diferentes en un solo script, por eso se agrupan y no existen los scripts del 61 al 70</t>
+    </r>
+  </si>
+  <si>
+    <t>Creacion de miembro con correo invalido</t>
+  </si>
+  <si>
+    <t>Creacion de miembro con Nombre corto</t>
+  </si>
+  <si>
+    <t>Creacion de miembro con Note con saltos de linea</t>
+  </si>
+  <si>
+    <t>Creacion de miembros con caracteres invalidos en el correo</t>
+  </si>
+  <si>
+    <t>Creacion de miembro con nombre muy largo</t>
+  </si>
+  <si>
+    <t>Creacion de miembro con correo con muchos caracteres</t>
+  </si>
+  <si>
+    <t>Creacion de miembro con correo sin arroba</t>
   </si>
 </sst>
 </file>
@@ -294,10 +399,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -317,7 +422,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -616,22 +721,22 @@
   <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C92" sqref="C92:C101"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2"/>
-    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" style="2" customWidth="1"/>
-    <col min="5" max="6" width="44.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="2"/>
+    <col min="2" max="2" width="25.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="44.83203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="2"/>
+    <col min="8" max="16384" width="11.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,467 +759,881 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B74" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B75" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B76" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B78" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B79" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>91</v>
       </c>
-      <c r="B92" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92" s="3" t="s">
+      <c r="B92" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C92" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="D92" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E92" s="2" t="s">
@@ -1124,13 +1643,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>92</v>
       </c>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
       <c r="E93" s="2" t="s">
         <v>29</v>
       </c>
@@ -1138,13 +1657,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>93</v>
       </c>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
       <c r="E94" s="2" t="s">
         <v>30</v>
       </c>
@@ -1152,13 +1671,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>94</v>
       </c>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
       <c r="E95" s="2" t="s">
         <v>31</v>
       </c>
@@ -1166,13 +1685,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>95</v>
       </c>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
       <c r="E96" s="2" t="s">
         <v>32</v>
       </c>
@@ -1180,13 +1699,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>96</v>
       </c>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
       <c r="E97" s="2" t="s">
         <v>33</v>
       </c>
@@ -1194,13 +1713,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>97</v>
       </c>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
       <c r="E98" s="2" t="s">
         <v>34</v>
       </c>
@@ -1208,13 +1727,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>98</v>
       </c>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
       <c r="E99" s="2" t="s">
         <v>35</v>
       </c>
@@ -1222,13 +1741,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>99</v>
       </c>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
       <c r="E100" s="2" t="s">
         <v>36</v>
       </c>
@@ -1236,13 +1755,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>100</v>
       </c>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
       <c r="E101" s="2" t="s">
         <v>37</v>
       </c>
@@ -1250,7 +1769,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -1260,7 +1779,7 @@
       <c r="C102" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D102" s="4" t="s">
+      <c r="D102" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E102" s="2" t="s">
@@ -1270,7 +1789,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -1280,7 +1799,7 @@
       <c r="C103" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D103" s="4" t="s">
+      <c r="D103" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E103" s="2" t="s">
@@ -1290,7 +1809,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -1300,7 +1819,7 @@
       <c r="C104" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D104" s="4" t="s">
+      <c r="D104" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E104" s="2" t="s">
@@ -1310,7 +1829,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -1320,7 +1839,7 @@
       <c r="C105" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D105" s="4" t="s">
+      <c r="D105" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E105" s="2" t="s">
@@ -1330,7 +1849,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -1340,7 +1859,7 @@
       <c r="C106" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D106" s="4" t="s">
+      <c r="D106" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E106" s="2" t="s">
@@ -1353,7 +1872,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -1363,7 +1882,7 @@
       <c r="C107" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="D107" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E107" s="2" t="s">
@@ -1373,7 +1892,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -1383,7 +1902,7 @@
       <c r="C108" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D108" s="4" t="s">
+      <c r="D108" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E108" s="2" t="s">
@@ -1396,7 +1915,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -1406,7 +1925,7 @@
       <c r="C109" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D109" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E109" s="2" t="s">
@@ -1419,7 +1938,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -1429,7 +1948,7 @@
       <c r="C110" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D110" s="4" t="s">
+      <c r="D110" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E110" s="2" t="s">
@@ -1439,7 +1958,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -1449,7 +1968,7 @@
       <c r="C111" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D111" s="4" t="s">
+      <c r="D111" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E111" s="2" t="s">
@@ -1459,7 +1978,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -1469,7 +1988,7 @@
       <c r="C112" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D112" s="4" t="s">
+      <c r="D112" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E112" s="2" t="s">
@@ -1479,7 +1998,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -1489,7 +2008,7 @@
       <c r="C113" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D113" s="4" t="s">
+      <c r="D113" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E113" s="2" t="s">
@@ -1499,7 +2018,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -1509,7 +2028,7 @@
       <c r="C114" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D114" s="4" t="s">
+      <c r="D114" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E114" s="2" t="s">
@@ -1519,7 +2038,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -1529,7 +2048,7 @@
       <c r="C115" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D115" s="4" t="s">
+      <c r="D115" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E115" s="2" t="s">
@@ -1542,7 +2061,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -1552,7 +2071,7 @@
       <c r="C116" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D116" s="4" t="s">
+      <c r="D116" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E116" s="2" t="s">
@@ -1562,7 +2081,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -1572,7 +2091,7 @@
       <c r="C117" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D117" s="4" t="s">
+      <c r="D117" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E117" s="2" t="s">
@@ -1585,7 +2104,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -1595,7 +2114,7 @@
       <c r="C118" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D118" s="4" t="s">
+      <c r="D118" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E118" s="2" t="s">
@@ -1605,7 +2124,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -1615,7 +2134,7 @@
       <c r="C119" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D119" s="4" t="s">
+      <c r="D119" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E119" s="2" t="s">
@@ -1625,7 +2144,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -1635,7 +2154,7 @@
       <c r="C120" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D120" s="4" t="s">
+      <c r="D120" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E120" s="2" t="s">
@@ -1645,7 +2164,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -1655,7 +2174,7 @@
       <c r="C121" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D121" s="4" t="s">
+      <c r="D121" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E121" s="2" t="s">
@@ -1666,10 +2185,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B92:B101"/>
     <mergeCell ref="C92:C101"/>
     <mergeCell ref="D92:D101"/>
+    <mergeCell ref="C62:C71"/>
+    <mergeCell ref="B62:B71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adicionar los pimeros treinta escnarios conforme a lo solicitado en la semana 7.
</commit_message>
<xml_diff>
--- a/Informe Semana 7.xlsx
+++ b/Informe Semana 7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresmartincantorurrego/Desktop/MAESTRIA/SEMESTRE 1/CICLO 2/PRUEBAS AUTOMATIZADAS /proyecto/semana5-pruebas-automatizadas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\mastertrack\pruebas\semana5-pruebas-automatizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1BDBFF-0617-734F-A106-F3A1B07D3986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7B13CB-F7A1-4619-A742-60A9351BBBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41340" yWindow="500" windowWidth="29660" windowHeight="20500" xr2:uid="{21504B3F-757C-4B36-B248-990E3DFEA9E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21504B3F-757C-4B36-B248-990E3DFEA9E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="153">
   <si>
     <t>ID</t>
   </si>
@@ -505,6 +505,27 @@
   </si>
   <si>
     <t>https://oalvareze.atlassian.net/browse/PAG-21</t>
+  </si>
+  <si>
+    <t>Javier Estupiñan</t>
+  </si>
+  <si>
+    <t>Escenario-prueba_1-10.js</t>
+  </si>
+  <si>
+    <t>Set a-priori, post function, enfoque positivo archivo json</t>
+  </si>
+  <si>
+    <t>Set a-priori, post function, enfoque negativo archivo json</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Escenario-prueba_11-20.js</t>
+  </si>
+  <si>
+    <t>Escenario-prueba_21-30.js</t>
   </si>
 </sst>
 </file>
@@ -563,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -586,6 +607,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,7 +628,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -903,22 +927,22 @@
   <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F87" sqref="F87"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22:C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="2"/>
-    <col min="2" max="2" width="25.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="50.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="44.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="2" customWidth="1"/>
+    <col min="5" max="6" width="44.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="11.5" style="2"/>
+    <col min="8" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -941,157 +965,411 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="8"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="8"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="8"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="8"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="8"/>
+      <c r="C7" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="8"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="8"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="8"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="8"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="8"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="8"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="8"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="8"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="8"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="8"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="8"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="8"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="8"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="8"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="8"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="8"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="8"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="8"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B31" s="8"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1112,7 +1390,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1127,7 +1405,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1142,7 +1420,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1157,7 +1435,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1172,7 +1450,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1187,7 +1465,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1202,7 +1480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1217,7 +1495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1232,7 +1510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1247,7 +1525,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1267,7 +1545,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1287,7 +1565,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1307,7 +1585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1327,7 +1605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1347,7 +1625,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1367,7 +1645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1387,7 +1665,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1407,7 +1685,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1427,7 +1705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1447,7 +1725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1467,7 +1745,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1487,7 +1765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1507,7 +1785,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1527,7 +1805,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1547,7 +1825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1567,7 +1845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1587,7 +1865,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1607,7 +1885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1627,7 +1905,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1647,7 +1925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -1667,7 +1945,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -1683,7 +1961,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -1699,7 +1977,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1715,7 +1993,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -1731,7 +2009,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -1747,7 +2025,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -1763,7 +2041,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -1779,7 +2057,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -1795,7 +2073,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -1811,7 +2089,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -1831,7 +2109,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -1851,7 +2129,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -1871,7 +2149,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -1891,7 +2169,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -1911,7 +2189,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -1931,7 +2209,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -1951,7 +2229,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -1971,7 +2249,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -1991,7 +2269,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -2011,7 +2289,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -2031,7 +2309,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -2051,7 +2329,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -2071,7 +2349,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -2091,7 +2369,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -2111,7 +2389,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -2131,7 +2409,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -2151,7 +2429,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -2171,7 +2449,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -2194,7 +2472,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -2214,7 +2492,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -2234,7 +2512,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -2248,7 +2526,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -2262,7 +2540,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -2276,7 +2554,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -2290,7 +2568,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -2304,7 +2582,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -2318,7 +2596,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -2332,7 +2610,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -2346,7 +2624,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -2360,7 +2638,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -2380,7 +2658,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -2400,7 +2678,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -2420,7 +2698,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -2440,7 +2718,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -2463,7 +2741,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -2483,7 +2761,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -2506,7 +2784,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -2529,7 +2807,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -2549,7 +2827,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -2569,7 +2847,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -2589,7 +2867,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -2609,7 +2887,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -2629,7 +2907,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -2652,7 +2930,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -2672,7 +2950,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -2695,7 +2973,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -2715,7 +2993,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -2735,7 +3013,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -2755,7 +3033,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -2776,7 +3054,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="15">
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="C12:C21"/>
+    <mergeCell ref="C22:C31"/>
+    <mergeCell ref="B12:B21"/>
+    <mergeCell ref="B22:B31"/>
+    <mergeCell ref="B2:B11"/>
     <mergeCell ref="C32:C41"/>
     <mergeCell ref="D32:D41"/>
     <mergeCell ref="B32:B41"/>
@@ -2787,5 +3072,6 @@
     <mergeCell ref="B62:B71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>